<commit_message>
Chapter 12 and 13 checked
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="73">
   <si>
     <t>Chapter</t>
   </si>
@@ -220,6 +220,33 @@
   </si>
   <si>
     <t>color and points differences | both graphs</t>
+  </si>
+  <si>
+    <t>MVAfactcarm</t>
+  </si>
+  <si>
+    <t>MVAfacthous</t>
+  </si>
+  <si>
+    <t>doesn't match | graph 4: mirrored image</t>
+  </si>
+  <si>
+    <t>MVAclus8p</t>
+  </si>
+  <si>
+    <t>slight differences | first graph</t>
+  </si>
+  <si>
+    <t>MVAclusbank</t>
+  </si>
+  <si>
+    <t>graphs don't match</t>
+  </si>
+  <si>
+    <t>MVAclusfood</t>
+  </si>
+  <si>
+    <t>MVAclusbh</t>
   </si>
 </sst>
 </file>
@@ -428,67 +455,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="93">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1759,11 +1726,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2362,6 +2329,216 @@
       <c r="A18" s="1">
         <v>12</v>
       </c>
+      <c r="B18" s="1">
+        <v>2159</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2159</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1398</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1211</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1211</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1672</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1201</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1201</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1664</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1202</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1202</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1665</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1205</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1205</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1667</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1204</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1204</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1666</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:I2"/>
@@ -2374,13 +2551,13 @@
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="containsText" dxfId="98" priority="1" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="2" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Chapters 16 and 17 checked
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="95">
   <si>
     <t>Chapter</t>
   </si>
@@ -285,7 +285,34 @@
     <t>MVAcancarm</t>
   </si>
   <si>
-    <t>doesn't match, check name in book (typo)</t>
+    <t>doesn't match +  (typo book)</t>
+  </si>
+  <si>
+    <t>MVAMDScity1</t>
+  </si>
+  <si>
+    <t>09.09.2016</t>
+  </si>
+  <si>
+    <t>MVAMDScity2</t>
+  </si>
+  <si>
+    <t>MVAmdscarm</t>
+  </si>
+  <si>
+    <t>MVAMDSpooladj</t>
+  </si>
+  <si>
+    <t>MVAMDSnonmstart</t>
+  </si>
+  <si>
+    <t>MVAnmdscar1</t>
+  </si>
+  <si>
+    <t>MVAnmdscar2</t>
+  </si>
+  <si>
+    <t>MVAnmdscar3</t>
   </si>
 </sst>
 </file>
@@ -448,6 +475,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -459,15 +495,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="25">
@@ -497,7 +524,187 @@
     <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="78">
+  <dxfs count="96">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1618,11 +1825,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1640,33 +1847,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="10" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="10"/>
+      <c r="I1" s="13"/>
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1726,7 +1933,7 @@
       <c r="J3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="9" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1796,7 +2003,7 @@
       <c r="J5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="8" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1831,7 +2038,7 @@
       <c r="J6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1971,7 +2178,7 @@
       <c r="J10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2041,7 +2248,7 @@
       <c r="J12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2076,7 +2283,7 @@
       <c r="J13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="9" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2286,7 +2493,7 @@
       <c r="J19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="9" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2356,7 +2563,7 @@
       <c r="J21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K21" s="9" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2461,7 +2668,7 @@
       <c r="J24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2496,7 +2703,7 @@
       <c r="J25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K25" s="14" t="s">
+      <c r="K25" s="10" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2566,7 +2773,7 @@
       <c r="J27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="13" t="s">
+      <c r="K27" s="9" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2601,7 +2808,7 @@
       <c r="J28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K28" s="13" t="s">
+      <c r="K28" s="9" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2671,7 +2878,7 @@
       <c r="J30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K30" s="13" t="s">
+      <c r="K30" s="9" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2741,8 +2948,293 @@
       <c r="J32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K32" s="13" t="s">
+      <c r="K32" s="9" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>17</v>
+      </c>
+      <c r="B33" s="1">
+        <v>930</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="1">
+        <v>930</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1">
+        <v>462</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>17</v>
+      </c>
+      <c r="B34" s="1">
+        <v>931</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="1">
+        <v>931</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="1">
+        <v>431</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>17</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1214</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1214</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1687</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>17</v>
+      </c>
+      <c r="B36" s="1">
+        <v>933</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="1">
+        <v>933</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="1">
+        <v>318</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>17</v>
+      </c>
+      <c r="B37" s="1">
+        <v>932</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="1">
+        <v>932</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="1">
+        <v>659</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>17</v>
+      </c>
+      <c r="B38" s="1">
+        <v>934</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="1">
+        <v>934</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="1">
+        <v>482</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>17</v>
+      </c>
+      <c r="B39" s="1">
+        <v>935</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="1">
+        <v>935</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="1">
+        <v>660</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>17</v>
+      </c>
+      <c r="B40" s="1">
+        <v>936</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="1">
+        <v>936</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="1">
+        <v>661</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2756,13 +3248,13 @@
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Transfering to ToDo, i.e. adding matlab code to folders from MVA-Ready. Matlab codes but not plots, because the plots from matlab should be as much similar as possible to the plots produced by R, i.e. the reference are the R graphics, not the old matlab graphics.
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="71955" yWindow="9825" windowWidth="25605" windowHeight="14895" tabRatio="500"/>
+    <workbookView xWindow="71955" yWindow="9825" windowWidth="25605" windowHeight="14895" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="118">
   <si>
     <t>Chapter</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Git vs. Slides</t>
   </si>
   <si>
-    <t>Git vs Book</t>
-  </si>
-  <si>
     <t>yaml.load_file("/Users/PetraB/GitHub/MVA-ToDo/QID-1225-MVApcasimu/Metainfo.txt")</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>08.09.2016</t>
   </si>
   <si>
-    <t>Color and shape of the points do not correspond</t>
-  </si>
-  <si>
     <t>MVAnpcafood</t>
   </si>
   <si>
@@ -180,9 +174,6 @@
     <t>MVAnpcahous</t>
   </si>
   <si>
-    <t>color differences | second graph</t>
-  </si>
-  <si>
     <t>MVAnpcahousi</t>
   </si>
   <si>
@@ -252,12 +243,6 @@
     <t>MVAaerbh</t>
   </si>
   <si>
-    <t>color differences, can not find table 14.1</t>
-  </si>
-  <si>
-    <t>can not find table 14.2</t>
-  </si>
-  <si>
     <t>signs of the data don't match</t>
   </si>
   <si>
@@ -373,6 +358,30 @@
   </si>
   <si>
     <t>esthetic differences, name in github: MVAbankruptcydis</t>
+  </si>
+  <si>
+    <t>MVACARTGiniTree1</t>
+  </si>
+  <si>
+    <t>MVACARTTwoingTree1</t>
+  </si>
+  <si>
+    <t>MVAppsib</t>
+  </si>
+  <si>
+    <t>can't find figure 20.35</t>
+  </si>
+  <si>
+    <t>esthetic differences | second graph</t>
+  </si>
+  <si>
+    <t>can't find table 14.2</t>
+  </si>
+  <si>
+    <t>color differences, can't find table 14.1</t>
+  </si>
+  <si>
+    <t>Git (R) vs Book</t>
   </si>
 </sst>
 </file>
@@ -584,97 +593,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="90">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="81">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1825,11 +1744,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1893,10 +1812,10 @@
         <v>5</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>38</v>
@@ -1922,7 +1841,7 @@
         <v>475</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>9</v>
@@ -1931,10 +1850,10 @@
         <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1966,13 +1885,13 @@
         <v>9</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>11</v>
       </c>
@@ -1992,7 +1911,7 @@
         <v>1670</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>9</v>
@@ -2001,10 +1920,10 @@
         <v>10</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2027,7 +1946,7 @@
         <v>1671</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>9</v>
@@ -2036,10 +1955,10 @@
         <v>10</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2062,7 +1981,7 @@
         <v>653</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>9</v>
@@ -2071,10 +1990,10 @@
         <v>10</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2085,7 +2004,7 @@
         <v>2511</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1">
         <v>2511</v>
@@ -2097,7 +2016,7 @@
         <v>1669</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>9</v>
@@ -2106,10 +2025,10 @@
         <v>10</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2120,7 +2039,7 @@
         <v>1048</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1">
         <v>1048</v>
@@ -2141,7 +2060,7 @@
         <v>9</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>37</v>
@@ -2155,7 +2074,7 @@
         <v>1118</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" s="1">
         <v>1118</v>
@@ -2167,7 +2086,7 @@
         <v>1239</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>9</v>
@@ -2176,10 +2095,10 @@
         <v>10</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2190,7 +2109,7 @@
         <v>1117</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1">
         <v>1117</v>
@@ -2211,10 +2130,10 @@
         <v>10</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2225,7 +2144,7 @@
         <v>1215</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1">
         <v>1215</v>
@@ -2237,7 +2156,7 @@
         <v>654</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>9</v>
@@ -2246,10 +2165,10 @@
         <v>10</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2260,7 +2179,7 @@
         <v>1216</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1">
         <v>1216</v>
@@ -2272,7 +2191,7 @@
         <v>408</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>9</v>
@@ -2281,10 +2200,10 @@
         <v>10</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2295,7 +2214,7 @@
         <v>1115</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1">
         <v>1115</v>
@@ -2307,7 +2226,7 @@
         <v>655</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>9</v>
@@ -2316,7 +2235,7 @@
         <v>10</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>37</v>
@@ -2330,7 +2249,7 @@
         <v>1116</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1">
         <v>1116</v>
@@ -2342,7 +2261,7 @@
         <v>1674</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>9</v>
@@ -2351,7 +2270,7 @@
         <v>10</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>37</v>
@@ -2365,7 +2284,7 @@
         <v>949</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1">
         <v>949</v>
@@ -2377,7 +2296,7 @@
         <v>1675</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>9</v>
@@ -2386,10 +2305,10 @@
         <v>10</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2400,7 +2319,7 @@
         <v>986</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1">
         <v>986</v>
@@ -2412,7 +2331,7 @@
         <v>1673</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>9</v>
@@ -2421,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2435,7 +2354,7 @@
         <v>2159</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1">
         <v>2159</v>
@@ -2447,7 +2366,7 @@
         <v>1398</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>9</v>
@@ -2456,7 +2375,7 @@
         <v>10</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>37</v>
@@ -2470,7 +2389,7 @@
         <v>1211</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1">
         <v>1211</v>
@@ -2482,7 +2401,7 @@
         <v>1672</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>9</v>
@@ -2491,10 +2410,10 @@
         <v>9</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2505,7 +2424,7 @@
         <v>1201</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1">
         <v>1201</v>
@@ -2517,7 +2436,7 @@
         <v>1664</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>9</v>
@@ -2526,10 +2445,10 @@
         <v>10</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2540,7 +2459,7 @@
         <v>1202</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D21" s="1">
         <v>1202</v>
@@ -2552,7 +2471,7 @@
         <v>1665</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>9</v>
@@ -2561,10 +2480,10 @@
         <v>10</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2575,7 +2494,7 @@
         <v>1205</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D22" s="1">
         <v>1205</v>
@@ -2587,7 +2506,7 @@
         <v>1667</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>9</v>
@@ -2596,7 +2515,7 @@
         <v>10</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>37</v>
@@ -2610,7 +2529,7 @@
         <v>1204</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1">
         <v>1204</v>
@@ -2622,7 +2541,7 @@
         <v>1666</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>9</v>
@@ -2631,7 +2550,7 @@
         <v>10</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>37</v>
@@ -2645,7 +2564,7 @@
         <v>1209</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D24" s="1">
         <v>1209</v>
@@ -2657,7 +2576,7 @@
         <v>1733</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>9</v>
@@ -2666,10 +2585,10 @@
         <v>9</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -2680,7 +2599,7 @@
         <v>2454</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D25" s="1">
         <v>2454</v>
@@ -2692,7 +2611,7 @@
         <v>656</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>9</v>
@@ -2701,10 +2620,10 @@
         <v>10</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2715,7 +2634,7 @@
         <v>928</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D26" s="1">
         <v>928</v>
@@ -2727,7 +2646,7 @@
         <v>493</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>9</v>
@@ -2736,7 +2655,7 @@
         <v>10</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>37</v>
@@ -2750,7 +2669,7 @@
         <v>1208</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D27" s="1">
         <v>1208</v>
@@ -2762,7 +2681,7 @@
         <v>1692</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>9</v>
@@ -2771,10 +2690,10 @@
         <v>10</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2785,7 +2704,7 @@
         <v>2344</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D28" s="1">
         <v>2344</v>
@@ -2806,10 +2725,10 @@
         <v>9</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2820,7 +2739,7 @@
         <v>1072</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D29" s="1">
         <v>1072</v>
@@ -2841,10 +2760,10 @@
         <v>10</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2855,7 +2774,7 @@
         <v>1113</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D30" s="1">
         <v>1113</v>
@@ -2876,10 +2795,10 @@
         <v>10</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2890,7 +2809,7 @@
         <v>1073</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D31" s="1">
         <v>1073</v>
@@ -2911,10 +2830,10 @@
         <v>10</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2925,7 +2844,7 @@
         <v>2086</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D32" s="1">
         <v>2086</v>
@@ -2946,10 +2865,10 @@
         <v>10</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2960,7 +2879,7 @@
         <v>930</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D33" s="1">
         <v>930</v>
@@ -2981,10 +2900,10 @@
         <v>10</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2995,7 +2914,7 @@
         <v>931</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D34" s="1">
         <v>931</v>
@@ -3016,10 +2935,10 @@
         <v>10</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -3030,7 +2949,7 @@
         <v>1214</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D35" s="1">
         <v>1214</v>
@@ -3051,10 +2970,10 @@
         <v>10</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -3065,7 +2984,7 @@
         <v>933</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D36" s="1">
         <v>933</v>
@@ -3086,10 +3005,10 @@
         <v>10</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3100,7 +3019,7 @@
         <v>932</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D37" s="1">
         <v>932</v>
@@ -3121,10 +3040,10 @@
         <v>10</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -3135,7 +3054,7 @@
         <v>934</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D38" s="1">
         <v>934</v>
@@ -3147,7 +3066,7 @@
         <v>482</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>9</v>
@@ -3156,7 +3075,7 @@
         <v>10</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>37</v>
@@ -3170,7 +3089,7 @@
         <v>935</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D39" s="1">
         <v>935</v>
@@ -3191,10 +3110,10 @@
         <v>10</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3205,7 +3124,7 @@
         <v>936</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D40" s="1">
         <v>936</v>
@@ -3226,10 +3145,10 @@
         <v>10</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -3240,7 +3159,7 @@
         <v>757</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D41" s="1">
         <v>757</v>
@@ -3261,10 +3180,10 @@
         <v>9</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3275,7 +3194,7 @@
         <v>1229</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D42" s="1">
         <v>1229</v>
@@ -3296,10 +3215,10 @@
         <v>9</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -3310,7 +3229,7 @@
         <v>1227</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D43" s="1">
         <v>1227</v>
@@ -3331,10 +3250,10 @@
         <v>9</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -3345,7 +3264,7 @@
         <v>1226</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D44" s="1">
         <v>1226</v>
@@ -3366,10 +3285,10 @@
         <v>9</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -3380,7 +3299,7 @@
         <v>1268</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D45" s="1">
         <v>1268</v>
@@ -3401,7 +3320,7 @@
         <v>9</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>37</v>
@@ -3415,7 +3334,7 @@
         <v>2305</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D46" s="1">
         <v>2305</v>
@@ -3436,10 +3355,10 @@
         <v>9</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -3450,7 +3369,7 @@
         <v>2154</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D47" s="1">
         <v>2154</v>
@@ -3462,7 +3381,7 @@
         <v>2153</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>9</v>
@@ -3471,7 +3390,7 @@
         <v>9</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>37</v>
@@ -3485,7 +3404,7 @@
         <v>1234</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D48" s="1">
         <v>1234</v>
@@ -3506,10 +3425,10 @@
         <v>9</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3520,7 +3439,7 @@
         <v>1233</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D49" s="1">
         <v>1233</v>
@@ -3541,10 +3460,10 @@
         <v>9</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3555,7 +3474,7 @@
         <v>1964</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D50" s="1">
         <v>1964</v>
@@ -3576,10 +3495,10 @@
         <v>9</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3590,7 +3509,7 @@
         <v>1965</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D51" s="1">
         <v>1965</v>
@@ -3611,10 +3530,10 @@
         <v>9</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3625,7 +3544,7 @@
         <v>1966</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D52" s="1">
         <v>1966</v>
@@ -3646,7 +3565,7 @@
         <v>9</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>37</v>
@@ -3660,7 +3579,7 @@
         <v>1967</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D53" s="1">
         <v>1967</v>
@@ -3681,7 +3600,7 @@
         <v>9</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>37</v>
@@ -3695,7 +3614,7 @@
         <v>1968</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D54" s="1">
         <v>1968</v>
@@ -3716,7 +3635,7 @@
         <v>9</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>37</v>
@@ -3730,7 +3649,7 @@
         <v>1707</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D55" s="1">
         <v>1707</v>
@@ -3751,10 +3670,10 @@
         <v>9</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -3765,7 +3684,7 @@
         <v>1708</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D56" s="1">
         <v>1708</v>
@@ -3786,10 +3705,10 @@
         <v>9</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -3800,7 +3719,7 @@
         <v>1581</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D57" s="1">
         <v>1581</v>
@@ -3821,15 +3740,115 @@
         <v>9</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>20</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1709</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58" s="1">
+        <v>1709</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1713</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>20</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1710</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1710</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>20</v>
+      </c>
+      <c r="B60" s="1">
+        <v>904</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D60" s="1">
+        <v>904</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1696</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -3843,14 +3862,36 @@
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="80" priority="7" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="79" priority="8" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="78" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="containsText" dxfId="77" priority="4" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH("Ready",K64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="5" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH("ToDo",K64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="75" priority="6" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",K64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="cellIs" dxfId="74" priority="3" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="2" operator="containsText" text="esthetic differences">
+      <formula>NOT(ISERROR(SEARCH("esthetic differences",K1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="1" operator="containsText" text="'t">
+      <formula>NOT(ISERROR(SEARCH("'t",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3867,8 +3908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3976,17 +4017,17 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ToDo files from chapter 12  to   20
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="117">
   <si>
     <t>Chapter</t>
   </si>
@@ -48,9 +48,6 @@
     <t>transfered</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>ID github</t>
   </si>
   <si>
@@ -306,12 +303,6 @@
     <t>MVAreturns</t>
   </si>
   <si>
-    <t>MVAportfolIBMFord</t>
-  </si>
-  <si>
-    <t>esthetic differences, name in github: MVAportfol_IBM_Ford</t>
-  </si>
-  <si>
     <t>MVAportfol</t>
   </si>
   <si>
@@ -354,12 +345,6 @@
     <t>MVACARTBan2</t>
   </si>
   <si>
-    <t>MVAbancrupcydis</t>
-  </si>
-  <si>
-    <t>esthetic differences, name in github: MVAbankruptcydis</t>
-  </si>
-  <si>
     <t>MVACARTGiniTree1</t>
   </si>
   <si>
@@ -382,6 +367,18 @@
   </si>
   <si>
     <t>Git (R) vs Book</t>
+  </si>
+  <si>
+    <t>MVAportfol_IBM_Ford</t>
+  </si>
+  <si>
+    <t>esthetic differences, name in book: MVAportfolIBMFord</t>
+  </si>
+  <si>
+    <t>MVAbankruptcydis</t>
+  </si>
+  <si>
+    <t>esthetic differences, name in book: MVAbancrupcydis</t>
   </si>
 </sst>
 </file>
@@ -593,7 +590,547 @@
     <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="147">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1867,8 +2404,8 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1890,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>
@@ -1914,31 +2451,31 @@
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1949,31 +2486,31 @@
         <v>1114</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>1114</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1">
         <v>475</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1984,31 +2521,31 @@
         <v>1225</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>1225</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1">
         <v>1242</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2019,31 +2556,31 @@
         <v>945</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1">
         <v>945</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1">
         <v>1670</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2054,31 +2591,31 @@
         <v>948</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>948</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1">
         <v>1671</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2089,31 +2626,31 @@
         <v>1223</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1">
         <v>1223</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1">
         <v>653</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2124,31 +2661,31 @@
         <v>2511</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1">
         <v>2511</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1">
         <v>1669</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2159,31 +2696,31 @@
         <v>1048</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1">
         <v>1048</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2194,31 +2731,31 @@
         <v>1118</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1">
         <v>1118</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1">
         <v>1239</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2229,31 +2766,31 @@
         <v>1117</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1">
         <v>1117</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2264,31 +2801,31 @@
         <v>1215</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1">
         <v>1215</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1">
         <v>654</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2299,31 +2836,31 @@
         <v>1216</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1">
         <v>1216</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="1">
         <v>408</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2334,31 +2871,31 @@
         <v>1115</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1">
         <v>1115</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="1">
         <v>655</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2369,31 +2906,31 @@
         <v>1116</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1">
         <v>1116</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="1">
         <v>1674</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2404,31 +2941,31 @@
         <v>949</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1">
         <v>949</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1">
         <v>1675</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2439,31 +2976,31 @@
         <v>986</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="1">
         <v>986</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="1">
         <v>1673</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2474,31 +3011,31 @@
         <v>2159</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1">
         <v>2159</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="1">
         <v>1398</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2509,31 +3046,31 @@
         <v>1211</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="1">
         <v>1211</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" s="1">
         <v>1672</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2544,31 +3081,31 @@
         <v>1201</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1">
         <v>1201</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="1">
         <v>1664</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2579,31 +3116,31 @@
         <v>1202</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1">
         <v>1202</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="1">
         <v>1665</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2614,31 +3151,31 @@
         <v>1205</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="1">
         <v>1205</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" s="1">
         <v>1667</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2649,31 +3186,31 @@
         <v>1204</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1">
         <v>1204</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" s="1">
         <v>1666</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2684,31 +3221,31 @@
         <v>1209</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D24" s="1">
         <v>1209</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" s="1">
         <v>1733</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -2719,31 +3256,31 @@
         <v>2454</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="1">
         <v>2454</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" s="1">
         <v>656</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2754,31 +3291,31 @@
         <v>928</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="1">
         <v>928</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" s="1">
         <v>493</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2789,31 +3326,31 @@
         <v>1208</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1">
         <v>1208</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" s="1">
         <v>1692</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2824,31 +3361,31 @@
         <v>2344</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1">
         <v>2344</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="1">
         <v>1701</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2859,31 +3396,31 @@
         <v>1072</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="1">
         <v>1072</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" s="1">
         <v>428</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2894,31 +3431,31 @@
         <v>1113</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="1">
         <v>1113</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" s="1">
         <v>510</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2929,31 +3466,31 @@
         <v>1073</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D31" s="1">
         <v>1073</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" s="1">
         <v>658</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2964,31 +3501,31 @@
         <v>2086</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="1">
         <v>2086</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" s="1">
         <v>2087</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2999,31 +3536,31 @@
         <v>930</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="1">
         <v>930</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" s="1">
         <v>462</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -3034,31 +3571,31 @@
         <v>931</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D34" s="1">
         <v>931</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" s="1">
         <v>431</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -3069,31 +3606,31 @@
         <v>1214</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D35" s="1">
         <v>1214</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" s="1">
         <v>1687</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -3104,31 +3641,31 @@
         <v>933</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D36" s="1">
         <v>933</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" s="1">
         <v>318</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3139,31 +3676,31 @@
         <v>932</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D37" s="1">
         <v>932</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" s="1">
         <v>659</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -3174,31 +3711,31 @@
         <v>934</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="1">
         <v>934</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" s="1">
         <v>482</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K38" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -3209,31 +3746,31 @@
         <v>935</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" s="1">
         <v>935</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" s="1">
         <v>660</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3244,31 +3781,31 @@
         <v>936</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D40" s="1">
         <v>936</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40" s="1">
         <v>661</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -3279,31 +3816,31 @@
         <v>757</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" s="1">
         <v>757</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F41" s="1">
         <v>1685</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3314,31 +3851,31 @@
         <v>1229</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="1">
         <v>1229</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" s="1">
         <v>1689</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -3349,31 +3886,31 @@
         <v>1227</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="D43" s="1">
         <v>1227</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" s="1">
         <v>1697</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -3384,31 +3921,31 @@
         <v>1226</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D44" s="1">
         <v>1226</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44" s="1">
         <v>1688</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -3419,31 +3956,31 @@
         <v>1268</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D45" s="1">
         <v>1268</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -3454,31 +3991,31 @@
         <v>2305</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D46" s="1">
         <v>2305</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -3489,31 +4026,31 @@
         <v>2154</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D47" s="1">
         <v>2154</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" s="1">
         <v>2153</v>
       </c>
       <c r="G47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -3524,31 +4061,31 @@
         <v>1234</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D48" s="1">
         <v>1234</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F48" s="1">
         <v>1703</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3559,31 +4096,31 @@
         <v>1233</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D49" s="1">
         <v>1233</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3594,31 +4131,31 @@
         <v>1964</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D50" s="1">
         <v>1964</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3629,31 +4166,31 @@
         <v>1965</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D51" s="1">
         <v>1965</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3664,31 +4201,31 @@
         <v>1966</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D52" s="1">
         <v>1966</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3699,31 +4236,31 @@
         <v>1967</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D53" s="1">
         <v>1967</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3734,31 +4271,31 @@
         <v>1968</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D54" s="1">
         <v>1968</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3769,31 +4306,31 @@
         <v>1707</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D55" s="1">
         <v>1707</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" s="1">
         <v>1711</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -3804,31 +4341,31 @@
         <v>1708</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D56" s="1">
         <v>1708</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" s="1">
         <v>1712</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -3839,31 +4376,31 @@
         <v>1581</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="D57" s="1">
         <v>1581</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" s="1">
         <v>1582</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -3874,31 +4411,31 @@
         <v>1709</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D58" s="1">
         <v>1709</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" s="1">
         <v>1713</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3909,31 +4446,31 @@
         <v>1710</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D59" s="1">
         <v>1710</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -3944,31 +4481,31 @@
         <v>904</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D60" s="1">
         <v>904</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" s="1">
         <v>1696</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3982,35 +4519,35 @@
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="containsText" dxfId="92" priority="7" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="146" priority="7" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="8" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="145" priority="8" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="144" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="89" priority="4" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="143" priority="4" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",K64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="142" priority="5" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",K64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="141" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",K64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="86" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="3" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="2" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="139" priority="2" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH("esthetic differences",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="1" operator="containsText" text="'t">
+    <cfRule type="containsText" dxfId="138" priority="1" operator="containsText" text="'t">
       <formula>NOT(ISERROR(SEARCH("'t",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4042,15 +4579,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4058,31 +4595,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4090,25 +4627,25 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4116,38 +4653,38 @@
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chapter 7 corrected + chapter 8 and 9
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="220">
   <si>
     <t>Chapter</t>
   </si>
@@ -542,9 +542,6 @@
     <t>it doesn't match: table is not included in GitHub</t>
   </si>
   <si>
-    <t>it doesn't match: table not included in GitHub folder</t>
-  </si>
-  <si>
     <t>MVAdenbank2</t>
   </si>
   <si>
@@ -638,13 +635,55 @@
     <t>MVAlrtest</t>
   </si>
   <si>
-    <t>nothing to compare</t>
-  </si>
-  <si>
     <t>MVAsimcibh</t>
   </si>
   <si>
-    <t>repeated</t>
+    <t>3;7</t>
+  </si>
+  <si>
+    <t>MVAresponsesurface</t>
+  </si>
+  <si>
+    <t>MVAcareffect</t>
+  </si>
+  <si>
+    <t>MVAboshousing</t>
+  </si>
+  <si>
+    <t>MVAdrug</t>
+  </si>
+  <si>
+    <t>MVAdrug3waysTab</t>
+  </si>
+  <si>
+    <t>MVAbankrupt</t>
+  </si>
+  <si>
+    <t>MVAdrugLogistic</t>
+  </si>
+  <si>
+    <t>esthetic differences: wider color spectrum in Book</t>
+  </si>
+  <si>
+    <t>tables don't match</t>
+  </si>
+  <si>
+    <t>one of the table doesn't match: Table 8.7</t>
+  </si>
+  <si>
+    <t>doesn't match : code doesn't run</t>
+  </si>
+  <si>
+    <t>MVAlassocontour</t>
+  </si>
+  <si>
+    <t>MVAlassoregress</t>
+  </si>
+  <si>
+    <t>MVAlassologit</t>
+  </si>
+  <si>
+    <t>MVAgrouplasso</t>
   </si>
 </sst>
 </file>
@@ -859,14 +898,14 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="45">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -882,11 +921,71 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1187,96 +1286,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1819,7 +1828,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -3934,35 +3943,35 @@
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="containsText" dxfId="38" priority="7" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="44" priority="7" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="8" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="42" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="41" priority="4" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",K64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="40" priority="5" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",K64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="39" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",K64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="'t">
+    <cfRule type="containsText" dxfId="38" priority="1" operator="containsText" text="'t">
       <formula>NOT(ISERROR(SEARCH("'t",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH("esthetic differences",K1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3978,11 +3987,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L74"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5536,9 +5545,9 @@
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>3</v>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="B46" s="1">
         <v>1615</v>
@@ -5565,7 +5574,7 @@
         <v>9</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>172</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -5576,7 +5585,7 @@
         <v>942</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D47" s="1">
         <v>942</v>
@@ -5605,7 +5614,7 @@
         <v>1207</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D48" s="1">
         <v>1207</v>
@@ -5620,7 +5629,7 @@
         <v>118</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>8</v>
@@ -5637,7 +5646,7 @@
         <v>1629</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D49" s="1">
         <v>1629</v>
@@ -5658,7 +5667,7 @@
         <v>8</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -5669,7 +5678,7 @@
         <v>1199</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D50" s="1">
         <v>1199</v>
@@ -5701,7 +5710,7 @@
         <v>1200</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D51" s="1">
         <v>1200</v>
@@ -5722,7 +5731,7 @@
         <v>8</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -5733,7 +5742,7 @@
         <v>1267</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D52" s="1">
         <v>1267</v>
@@ -5754,7 +5763,7 @@
         <v>8</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -5765,7 +5774,7 @@
         <v>1478</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D53" s="1">
         <v>1478</v>
@@ -5797,7 +5806,7 @@
         <v>1235</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D54" s="1">
         <v>1235</v>
@@ -5829,7 +5838,7 @@
         <v>1481</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D55" s="1">
         <v>1481</v>
@@ -5861,7 +5870,7 @@
         <v>1264</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D56" s="1">
         <v>1264</v>
@@ -5879,7 +5888,7 @@
         <v>8</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>36</v>
@@ -5893,7 +5902,7 @@
         <v>1492</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D57" s="1">
         <v>1492</v>
@@ -5925,7 +5934,7 @@
         <v>1482</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D58" s="1">
         <v>1482</v>
@@ -5946,7 +5955,7 @@
         <v>9</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -5957,7 +5966,7 @@
         <v>1479</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D59" s="1">
         <v>1479</v>
@@ -5978,7 +5987,7 @@
         <v>8</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -5989,7 +5998,7 @@
         <v>1477</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D60" s="1">
         <v>1477</v>
@@ -6021,7 +6030,7 @@
         <v>1480</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D61" s="1">
         <v>1480</v>
@@ -6053,7 +6062,7 @@
         <v>1212</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D62" s="1">
         <v>1212</v>
@@ -6085,7 +6094,7 @@
         <v>1230</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D63" s="1">
         <v>1230</v>
@@ -6106,7 +6115,7 @@
         <v>8</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -6117,7 +6126,7 @@
         <v>1654</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D64" s="1">
         <v>1654</v>
@@ -6141,7 +6150,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>4</v>
       </c>
@@ -6149,7 +6158,7 @@
         <v>1653</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D65" s="1">
         <v>1653</v>
@@ -6173,7 +6182,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>5</v>
       </c>
@@ -6181,7 +6190,7 @@
         <v>1652</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D66" s="1">
         <v>1652</v>
@@ -6202,10 +6211,10 @@
         <v>8</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>7</v>
       </c>
@@ -6213,7 +6222,7 @@
         <v>2426</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D67" s="1">
         <v>2426</v>
@@ -6237,7 +6246,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>7</v>
       </c>
@@ -6245,7 +6254,7 @@
         <v>1660</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D68" s="1">
         <v>1660</v>
@@ -6266,10 +6275,10 @@
         <v>8</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>7</v>
       </c>
@@ -6277,7 +6286,7 @@
         <v>1661</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D69" s="1">
         <v>1661</v>
@@ -6295,10 +6304,10 @@
         <v>9</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>7</v>
       </c>
@@ -6306,7 +6315,7 @@
         <v>1659</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D70" s="1">
         <v>1659</v>
@@ -6327,10 +6336,10 @@
         <v>8</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>7</v>
       </c>
@@ -6338,7 +6347,7 @@
         <v>941</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D71" s="1">
         <v>941</v>
@@ -6362,7 +6371,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>7</v>
       </c>
@@ -6370,7 +6379,7 @@
         <v>1684</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D72" s="1">
         <v>1684</v>
@@ -6391,68 +6400,391 @@
         <v>8</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>7</v>
       </c>
       <c r="B73" s="1">
-        <v>1615</v>
+        <v>1682</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="D73" s="1">
-        <v>1615</v>
+        <v>1682</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F73" s="1">
-        <v>499</v>
+        <v>425</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="H73" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="I73" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="L73" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B74" s="1">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D74" s="1">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F74" s="1">
-        <v>425</v>
+        <v>641</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="H74" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="I74" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>204</v>
+        <v>8</v>
+      </c>
+      <c r="K74" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>8</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1532</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1532</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="1">
+        <v>1678</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>8</v>
+      </c>
+      <c r="B76" s="1">
+        <v>2427</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D76" s="1">
+        <v>2427</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="1">
+        <v>1677</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>8</v>
+      </c>
+      <c r="B77" s="1">
+        <v>1046</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1046</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="1">
+        <v>642</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>8</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1716</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1716</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>8</v>
+      </c>
+      <c r="B79" s="1">
+        <v>2455</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D79" s="1">
+        <v>2455</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="1">
+        <v>1676</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>8</v>
+      </c>
+      <c r="B80" s="1">
+        <v>1679</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1679</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1680</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>9</v>
+      </c>
+      <c r="B81" s="1">
+        <v>2963</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D81" s="1">
+        <v>2963</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>9</v>
+      </c>
+      <c r="B82" s="1">
+        <v>2555</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D82" s="1">
+        <v>2555</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>9</v>
+      </c>
+      <c r="B83" s="1">
+        <v>2527</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D83" s="1">
+        <v>2527</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>9</v>
+      </c>
+      <c r="B84" s="1">
+        <v>2525</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D84" s="1">
+        <v>2525</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -6464,81 +6796,136 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D1:J13 E14:J14 D15:J43 G45 D44:H44 J44 I44:I45 D46:J70 I71:J71 D75:J1048576 H72:J74 D70:F71 D73:D74 F73:F74 E72:E74">
-    <cfRule type="containsText" dxfId="29" priority="22" operator="containsText" text="Ready">
+  <conditionalFormatting sqref="D1:J13 E14:J14 D15:J43 G45 D44:H44 J44 I44:I45 D46:J70 I71:J71 D70:F71 G72:J72 D73 E72:E73 D79:F80 D85:J1048576 D82:E84 G84 J78:J84 D74:G78 F73:G73 I73:J77">
+    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",K6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",K6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",K6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K14 K16:K1048576">
-    <cfRule type="containsText" dxfId="23" priority="16" operator="containsText" text="'t">
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="'t">
       <formula>NOT(ISERROR(SEARCH("'t",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH("esthetic differences",K1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="20" priority="13" operator="containsText" text="'t">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="'t">
       <formula>NOT(ISERROR(SEARCH("'t",K15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH("esthetic differences",K15)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",E45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",E45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",E45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D71:H71 E72:E74 G72:G74">
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Ready">
+  <conditionalFormatting sqref="D71:H71">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D71)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D71)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D71)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D74 F74">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH("Ready",D74)))</formula>
+  <conditionalFormatting sqref="D73 F73">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH("Ready",D73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH("ToDo",D74)))</formula>
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH("ToDo",D73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",D74)))</formula>
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",D73)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E81">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH("Ready",E81)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH("ToDo",E81)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G79:G83">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH("Ready",G79)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH("ToDo",G79)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",G79)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F81:F84">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH("Ready",F81)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH("ToDo",F81)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",F81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78:I84">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH("Ready",H78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH("ToDo",H78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",H78)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H73:H77">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH("Ready",H73)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH("ToDo",H73)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding boxcity to ToDo
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -863,13 +863,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -904,6 +904,96 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="45">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1171,96 +1261,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1834,7 +1834,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1852,33 +1852,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="15"/>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="12"/>
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>490</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>8</v>
@@ -4640,134 +4640,134 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:J13 E14:J14 D15:J43 G45 D44:H44 J44 I44:I45 D46:J70 I71:J71 D70:F71 G72:J72 D73 E72:E73 D79:F80 D85:J1048576 D82:E84 G84 J78:J84 D74:G78 F73:G73 I73:J77">
-    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="44" priority="37" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="43" priority="38" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="42" priority="39" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="41" priority="34" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",K6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="40" priority="35" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",K6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="39" priority="36" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",K6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K14 K16:K1048576">
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="'t">
+    <cfRule type="containsText" dxfId="38" priority="31" operator="containsText" text="'t">
       <formula>NOT(ISERROR(SEARCH("'t",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="37" priority="32" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH("esthetic differences",K1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="'t">
+    <cfRule type="containsText" dxfId="35" priority="28" operator="containsText" text="'t">
       <formula>NOT(ISERROR(SEARCH("'t",K15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="34" priority="29" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH("esthetic differences",K15)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="32" priority="22" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",E45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="31" priority="23" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",E45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="30" priority="24" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",E45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D71:H71">
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D71)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D71)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73 F73">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="26" priority="16" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="25" priority="17" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="24" priority="18" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",E81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",E81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",E81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79:G83">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",G79)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",G79)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",G79)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81:F84">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",F81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",F81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",F81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78:I84">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",H78)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",H78)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",H78)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4781,8 +4781,8 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4800,33 +4800,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="15"/>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="12"/>
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
@@ -6896,35 +6896,35 @@
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="containsText" dxfId="44" priority="7" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="41" priority="4" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",K64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",K64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",K64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="containsText" dxfId="38" priority="1" operator="containsText" text="'t">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="'t">
       <formula>NOT(ISERROR(SEARCH("'t",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH("esthetic differences",K1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
check Matlab vs R
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="219">
   <si>
     <t>Chapter</t>
   </si>
@@ -678,13 +678,16 @@
   </si>
   <si>
     <t>MVAdraftbank4</t>
+  </si>
+  <si>
+    <t>Matlab Check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -735,6 +738,13 @@
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -794,7 +804,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -820,8 +830,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -852,6 +863,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -867,11 +881,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="25" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -897,15 +911,16 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="25" builtinId="5"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="51">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -921,11 +936,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -986,156 +1001,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2035,11 +1900,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2050,40 +1915,40 @@
     <col min="4" max="5" width="12.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="12.375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="36.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="12.375" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="36.25" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="12"/>
+      <c r="I1" s="13"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+    <row r="2" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2111,8 +1976,11 @@
       <c r="L2" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2146,8 +2014,11 @@
       <c r="K3" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -2181,8 +2052,11 @@
       <c r="K4" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -2216,8 +2090,11 @@
       <c r="K5" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -2251,15 +2128,18 @@
       <c r="K6" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>1489</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="18" t="s">
         <v>120</v>
       </c>
       <c r="D7" s="1">
@@ -2287,7 +2167,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -2322,7 +2202,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -2357,7 +2237,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -2392,7 +2272,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -2427,7 +2307,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -2462,7 +2342,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -2497,7 +2377,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -2532,7 +2412,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -2567,7 +2447,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -4786,7 +4666,7 @@
         <v>1676</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>8</v>
@@ -4821,7 +4701,7 @@
         <v>1680</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>8</v>
@@ -4986,156 +4866,156 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="E14:J14 D15:J31 I44:I45 I71 D46:F71 H72:I72 D73 E72:E73 D79:F80 D85:J1048576 D82:E84 G84 D78:G78 F73 I73:I77 D74:F77 H46:I70 H44 D32:F44 H32:I43 D1:J13 J13:J28 J78:J84">
-    <cfRule type="containsText" dxfId="65" priority="43" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="50" priority="43" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="44" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="49" priority="44" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="45" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="48" priority="45" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="62" priority="40" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="47" priority="40" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",K6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="46" priority="41" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",K6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="42" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="45" priority="42" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",K6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K14 K16:K1048576">
-    <cfRule type="containsText" dxfId="59" priority="37" operator="containsText" text="'t">
+    <cfRule type="containsText" dxfId="44" priority="37" operator="containsText" text="'t">
       <formula>NOT(ISERROR(SEARCH("'t",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="43" priority="38" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH("esthetic differences",K1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="39" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="56" priority="34" operator="containsText" text="'t">
+    <cfRule type="containsText" dxfId="41" priority="34" operator="containsText" text="'t">
       <formula>NOT(ISERROR(SEARCH("'t",K15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="35" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="40" priority="35" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH("esthetic differences",K15)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="53" priority="28" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="38" priority="28" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",E45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="29" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="37" priority="29" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",E45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="30" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="36" priority="30" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",E45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D71:F71 H71">
-    <cfRule type="containsText" dxfId="50" priority="25" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="35" priority="25" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D71)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="26" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="34" priority="26" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D71)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="27" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73 F73">
-    <cfRule type="containsText" dxfId="47" priority="22" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="32" priority="22" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="23" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="31" priority="23" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="24" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="30" priority="24" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="containsText" dxfId="44" priority="19" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",E81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="20" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",E81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="21" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",E81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79:G83">
-    <cfRule type="containsText" dxfId="41" priority="16" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="26" priority="16" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",G79)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="17" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="25" priority="17" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",G79)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="24" priority="18" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",G79)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81:F84">
-    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",F81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",F81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",F81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78:I84">
-    <cfRule type="containsText" dxfId="35" priority="10" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",H78)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="11" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",H78)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",H78)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="32" priority="7" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="8" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:G77">
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",G32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",G32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",G32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32:J77">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",J32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",J32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",J32)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5157,7 +5037,7 @@
   <cols>
     <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" style="1"/>
-    <col min="3" max="3" width="21.875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="21.875" style="12" customWidth="1"/>
     <col min="4" max="5" width="12.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.375" style="1" customWidth="1"/>
@@ -5168,33 +5048,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="12"/>
+      <c r="I1" s="13"/>
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="16"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
@@ -5230,7 +5110,7 @@
       <c r="B3" s="1">
         <v>1114</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1">
@@ -5265,7 +5145,7 @@
       <c r="B4" s="1">
         <v>1225</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="12" t="s">
         <v>216</v>
       </c>
       <c r="D4" s="1">
@@ -5300,7 +5180,7 @@
       <c r="B5" s="1">
         <v>945</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1">
@@ -5335,7 +5215,7 @@
       <c r="B6" s="1">
         <v>948</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1">
@@ -5370,7 +5250,7 @@
       <c r="B7" s="1">
         <v>1223</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1">
@@ -5405,7 +5285,7 @@
       <c r="B8" s="1">
         <v>2511</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D8" s="1">
@@ -5440,7 +5320,7 @@
       <c r="B9" s="1">
         <v>1048</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D9" s="1">
@@ -5475,7 +5355,7 @@
       <c r="B10" s="1">
         <v>1118</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D10" s="1">
@@ -5510,7 +5390,7 @@
       <c r="B11" s="1">
         <v>1117</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="1">
@@ -5545,7 +5425,7 @@
       <c r="B12" s="1">
         <v>1215</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D12" s="1">
@@ -5580,7 +5460,7 @@
       <c r="B13" s="1">
         <v>1216</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="12" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="1">
@@ -5615,7 +5495,7 @@
       <c r="B14" s="1">
         <v>1115</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D14" s="1">
@@ -5650,7 +5530,7 @@
       <c r="B15" s="1">
         <v>1116</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="12" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="1">
@@ -5685,7 +5565,7 @@
       <c r="B16" s="1">
         <v>949</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="12" t="s">
         <v>53</v>
       </c>
       <c r="D16" s="1">
@@ -5720,7 +5600,7 @@
       <c r="B17" s="1">
         <v>986</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D17" s="1">
@@ -5755,7 +5635,7 @@
       <c r="B18" s="1">
         <v>2159</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="12" t="s">
         <v>55</v>
       </c>
       <c r="D18" s="1">
@@ -5790,7 +5670,7 @@
       <c r="B19" s="1">
         <v>1211</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="1">
@@ -5825,7 +5705,7 @@
       <c r="B20" s="1">
         <v>1201</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D20" s="1">
@@ -5860,7 +5740,7 @@
       <c r="B21" s="1">
         <v>1202</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D21" s="1">
@@ -5895,7 +5775,7 @@
       <c r="B22" s="1">
         <v>1205</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="12" t="s">
         <v>61</v>
       </c>
       <c r="D22" s="1">
@@ -5930,7 +5810,7 @@
       <c r="B23" s="1">
         <v>1204</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="12" t="s">
         <v>62</v>
       </c>
       <c r="D23" s="1">
@@ -5965,7 +5845,7 @@
       <c r="B24" s="1">
         <v>1209</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D24" s="1">
@@ -6000,7 +5880,7 @@
       <c r="B25" s="1">
         <v>2454</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D25" s="1">
@@ -6035,7 +5915,7 @@
       <c r="B26" s="1">
         <v>928</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="12" t="s">
         <v>64</v>
       </c>
       <c r="D26" s="1">
@@ -6070,7 +5950,7 @@
       <c r="B27" s="1">
         <v>1208</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D27" s="1">
@@ -6105,7 +5985,7 @@
       <c r="B28" s="1">
         <v>2344</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="12" t="s">
         <v>68</v>
       </c>
       <c r="D28" s="1">
@@ -6140,7 +6020,7 @@
       <c r="B29" s="1">
         <v>1072</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D29" s="1">
@@ -6175,7 +6055,7 @@
       <c r="B30" s="1">
         <v>1113</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="12" t="s">
         <v>71</v>
       </c>
       <c r="D30" s="1">
@@ -6210,7 +6090,7 @@
       <c r="B31" s="1">
         <v>1073</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D31" s="1">
@@ -6245,7 +6125,7 @@
       <c r="B32" s="1">
         <v>2086</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="12" t="s">
         <v>77</v>
       </c>
       <c r="D32" s="1">
@@ -6280,7 +6160,7 @@
       <c r="B33" s="1">
         <v>930</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="12" t="s">
         <v>79</v>
       </c>
       <c r="D33" s="1">
@@ -6315,7 +6195,7 @@
       <c r="B34" s="1">
         <v>931</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="12" t="s">
         <v>81</v>
       </c>
       <c r="D34" s="1">
@@ -6350,7 +6230,7 @@
       <c r="B35" s="1">
         <v>1214</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="12" t="s">
         <v>82</v>
       </c>
       <c r="D35" s="1">
@@ -6385,7 +6265,7 @@
       <c r="B36" s="1">
         <v>933</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="12" t="s">
         <v>83</v>
       </c>
       <c r="D36" s="1">
@@ -6420,7 +6300,7 @@
       <c r="B37" s="1">
         <v>932</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="12" t="s">
         <v>84</v>
       </c>
       <c r="D37" s="1">
@@ -6455,7 +6335,7 @@
       <c r="B38" s="1">
         <v>934</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="12" t="s">
         <v>85</v>
       </c>
       <c r="D38" s="1">
@@ -6490,7 +6370,7 @@
       <c r="B39" s="1">
         <v>935</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="12" t="s">
         <v>86</v>
       </c>
       <c r="D39" s="1">
@@ -6525,7 +6405,7 @@
       <c r="B40" s="1">
         <v>936</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="12" t="s">
         <v>87</v>
       </c>
       <c r="D40" s="1">
@@ -6560,7 +6440,7 @@
       <c r="B41" s="1">
         <v>757</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="12" t="s">
         <v>88</v>
       </c>
       <c r="D41" s="1">
@@ -6595,7 +6475,7 @@
       <c r="B42" s="1">
         <v>1229</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="12" t="s">
         <v>89</v>
       </c>
       <c r="D42" s="1">
@@ -6630,7 +6510,7 @@
       <c r="B43" s="1">
         <v>1227</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="12" t="s">
         <v>112</v>
       </c>
       <c r="D43" s="1">
@@ -6665,7 +6545,7 @@
       <c r="B44" s="1">
         <v>1226</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="12" t="s">
         <v>90</v>
       </c>
       <c r="D44" s="1">
@@ -6700,7 +6580,7 @@
       <c r="B45" s="1">
         <v>1268</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="12" t="s">
         <v>91</v>
       </c>
       <c r="D45" s="1">
@@ -6735,7 +6615,7 @@
       <c r="B46" s="1">
         <v>2305</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="12" t="s">
         <v>92</v>
       </c>
       <c r="D46" s="1">
@@ -6770,7 +6650,7 @@
       <c r="B47" s="1">
         <v>2154</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="12" t="s">
         <v>93</v>
       </c>
       <c r="D47" s="1">
@@ -6805,7 +6685,7 @@
       <c r="B48" s="1">
         <v>1234</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="12" t="s">
         <v>94</v>
       </c>
       <c r="D48" s="1">
@@ -6840,7 +6720,7 @@
       <c r="B49" s="1">
         <v>1233</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C49" s="12" t="s">
         <v>96</v>
       </c>
       <c r="D49" s="1">
@@ -6875,7 +6755,7 @@
       <c r="B50" s="1">
         <v>1964</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="12" t="s">
         <v>97</v>
       </c>
       <c r="D50" s="1">
@@ -6910,7 +6790,7 @@
       <c r="B51" s="1">
         <v>1965</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C51" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D51" s="1">
@@ -6945,7 +6825,7 @@
       <c r="B52" s="1">
         <v>1966</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="12" t="s">
         <v>99</v>
       </c>
       <c r="D52" s="1">
@@ -6980,7 +6860,7 @@
       <c r="B53" s="1">
         <v>1967</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C53" s="12" t="s">
         <v>100</v>
       </c>
       <c r="D53" s="1">
@@ -7015,7 +6895,7 @@
       <c r="B54" s="1">
         <v>1968</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="12" t="s">
         <v>101</v>
       </c>
       <c r="D54" s="1">
@@ -7050,7 +6930,7 @@
       <c r="B55" s="1">
         <v>1707</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="12" t="s">
         <v>102</v>
       </c>
       <c r="D55" s="1">
@@ -7085,7 +6965,7 @@
       <c r="B56" s="1">
         <v>1708</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D56" s="1">
@@ -7120,7 +7000,7 @@
       <c r="B57" s="1">
         <v>1581</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C57" s="12" t="s">
         <v>114</v>
       </c>
       <c r="D57" s="1">
@@ -7155,7 +7035,7 @@
       <c r="B58" s="1">
         <v>1709</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="12" t="s">
         <v>104</v>
       </c>
       <c r="D58" s="1">
@@ -7190,7 +7070,7 @@
       <c r="B59" s="1">
         <v>1710</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C59" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D59" s="1">
@@ -7225,7 +7105,7 @@
       <c r="B60" s="1">
         <v>904</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="12" t="s">
         <v>106</v>
       </c>
       <c r="D60" s="1">
@@ -7264,35 +7144,35 @@
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="containsText" dxfId="29" priority="7" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH("Ready",K64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",K64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",K64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="'t">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="'t">
       <formula>NOT(ISERROR(SEARCH("'t",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH("esthetic differences",K1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
R code checked, the quantlet is not yet ready.
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithupFiles\MVA-ToDo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="915" windowWidth="17655" windowHeight="5040" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="915" windowWidth="17655" windowHeight="5040" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Steps" sheetId="1" r:id="rId1"/>
     <sheet name="Chapters 1 to 9" sheetId="2" r:id="rId2"/>
     <sheet name="Chapters 10 to 20" sheetId="3" r:id="rId3"/>
+    <sheet name="New Quantlets" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Chapters 10 to 20'!$A$2:$I$2</definedName>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="224">
   <si>
     <t>Chapter</t>
   </si>
@@ -683,12 +689,22 @@
   <si>
     <t>new graph</t>
   </si>
+  <si>
+    <t>The output of the new codes (R and Matlab) corresponds to the figure  5 of the paper "The Dynamics of Implied Volatilities:
+A Common Principal Components Approach"</t>
+  </si>
+  <si>
+    <t>01.12.2016</t>
+  </si>
+  <si>
+    <t>MVAspecclustspiral</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -727,8 +743,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -757,6 +780,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0066"/>
         <bgColor rgb="FFFF0066"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -839,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -897,11 +932,546 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="82">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1775,12 +2345,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1822,7 +2395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1857,7 +2430,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2072,7 +2645,7 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="5.125" customWidth="1"/>
@@ -5326,12 +5899,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3:M65"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.125" customWidth="1"/>
     <col min="2" max="2" width="10.875" customWidth="1"/>
@@ -35310,212 +35883,212 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="E14:J14 D15:J31 I44:I45 I71 D46:F71 H72:I72 D73 E72:E73 D79:F80 D85:J1000 D82:E84 G84 D78:G78 F73 I73:I77 D74:F77 H46:I70 H44 D32:F44 H32:I43 D1:J13 J78:J84 J13:J28">
-    <cfRule type="containsText" dxfId="50" priority="1" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="81" priority="1" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(E14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:J14 D15:J31 I44:I45 I71 D46:F71 H72:I72 D73 E72:E73 D79:F80 D85:J1000 D82:E84 G84 D78:G78 F73 I73:I77 D74:F77 H46:I70 H44 D32:F44 H32:I43 D1:J13 J78:J84 J13:J28">
-    <cfRule type="containsText" dxfId="49" priority="2" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="80" priority="2" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(E14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:J14 D15:J31 I44:I45 I71 D46:F71 H72:I72 D73 E72:E73 D79:F80 D85:J1000 D82:E84 G84 D78:G78 F73 I73:I77 D74:F77 H46:I70 H44 D32:F44 H32:I43 D1:J13 J78:J84 J13:J28">
-    <cfRule type="containsText" dxfId="48" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="79" priority="3" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(E14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="47" priority="4" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="78" priority="4" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(K6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="46" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(K6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="45" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="76" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(K6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K14 K16:K1000">
-    <cfRule type="containsText" dxfId="44" priority="7" operator="containsText" text="t">
+    <cfRule type="containsText" dxfId="75" priority="7" operator="containsText" text="t">
       <formula>NOT(ISERROR(SEARCH(("t"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K14 K16:K1000">
-    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="74" priority="8" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH(("esthetic differences"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K14 K16:K1000">
-    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="9" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="41" priority="10" operator="containsText" text="t">
+    <cfRule type="containsText" dxfId="72" priority="10" operator="containsText" text="t">
       <formula>NOT(ISERROR(SEARCH(("t"),(K15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="40" priority="11" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="71" priority="11" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH(("esthetic differences"),(K15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="39" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="12" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="69" priority="13" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(E45))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="68" priority="14" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(E45))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="67" priority="15" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(E45))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D71:F71 H71">
-    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="66" priority="16" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(D71))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D71:F71 H71">
-    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="65" priority="17" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(D71))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D71:F71 H71">
-    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="64" priority="18" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(D71))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73 F73">
-    <cfRule type="containsText" dxfId="32" priority="19" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="63" priority="19" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(D73))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73 F73">
-    <cfRule type="containsText" dxfId="31" priority="20" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="62" priority="20" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(D73))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73 F73">
-    <cfRule type="containsText" dxfId="30" priority="21" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="61" priority="21" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(D73))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="containsText" dxfId="29" priority="22" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="60" priority="22" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(E81))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="59" priority="23" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(E81))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="58" priority="24" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(E81))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79:G83">
-    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="57" priority="25" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(G79))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79:G83">
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="56" priority="26" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(G79))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79:G83">
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="55" priority="27" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(G79))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81:F84">
-    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="54" priority="28" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(F81))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81:F84">
-    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="53" priority="29" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(F81))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81:F84">
-    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="52" priority="30" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(F81))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78:I84">
-    <cfRule type="containsText" dxfId="20" priority="31" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(H78))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78:I84">
-    <cfRule type="containsText" dxfId="19" priority="32" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(H78))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78:I84">
-    <cfRule type="containsText" dxfId="18" priority="33" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="49" priority="33" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(H78))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="17" priority="34" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="48" priority="34" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(H73))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="16" priority="35" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="47" priority="35" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(H73))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="15" priority="36" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="46" priority="36" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(H73))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:G77">
-    <cfRule type="containsText" dxfId="14" priority="37" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="45" priority="37" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(G32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:G77">
-    <cfRule type="containsText" dxfId="13" priority="38" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="44" priority="38" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(G32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:G77">
-    <cfRule type="containsText" dxfId="12" priority="39" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="43" priority="39" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(G32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32:J77">
-    <cfRule type="containsText" dxfId="11" priority="40" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(J32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32:J77">
-    <cfRule type="containsText" dxfId="10" priority="41" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(J32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32:J77">
-    <cfRule type="containsText" dxfId="9" priority="42" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(J32))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35528,12 +36101,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.125" customWidth="1"/>
     <col min="2" max="2" width="10.875" customWidth="1"/>
@@ -35544,7 +36117,9 @@
     <col min="8" max="8" width="8.875" customWidth="1"/>
     <col min="9" max="10" width="12.375" customWidth="1"/>
     <col min="11" max="11" width="36.25" customWidth="1"/>
-    <col min="12" max="26" width="10.875" customWidth="1"/>
+    <col min="12" max="12" width="10.875" customWidth="1"/>
+    <col min="13" max="13" width="53.25" customWidth="1"/>
+    <col min="14" max="26" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -35618,7 +36193,9 @@
       <c r="L2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="5"/>
+      <c r="M2" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -35933,7 +36510,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>11</v>
       </c>
@@ -35953,7 +36530,7 @@
         <v>38</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>38</v>
@@ -35961,15 +36538,16 @@
       <c r="I9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>45</v>
+      <c r="J9" s="23" t="s">
+        <v>222</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="M9" s="16" t="s">
+        <v>221</v>
+      </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
@@ -64861,48 +65439,104 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:J1000">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:J1000">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="38" priority="2" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:J1000">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64:K1000">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="36" priority="4" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(K64))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64:K1000">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(K64))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64:K1000">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(K64))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="t">
+    <cfRule type="containsText" dxfId="33" priority="7" operator="containsText" text="t">
       <formula>NOT(ISERROR(SEARCH(("t"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="32" priority="8" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH(("esthetic differences"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
       <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="25"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH("ToDo",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrected Matlab Codes - Metainfo checked.
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithupFiles\MVA-ToDo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="915" windowWidth="17655" windowHeight="5040" activeTab="3"/>
+    <workbookView xWindow="630" yWindow="915" windowWidth="17655" windowHeight="5040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Steps" sheetId="1" r:id="rId1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="224">
   <si>
     <t>Chapter</t>
   </si>
@@ -684,9 +679,6 @@
     <t>MVAgrouplasso</t>
   </si>
   <si>
-    <t>We tried to reproduce R-function in Matlab but it reads Fortran-Code</t>
-  </si>
-  <si>
     <t>new graph</t>
   </si>
   <si>
@@ -698,6 +690,9 @@
   </si>
   <si>
     <t>MVAspecclustspiral</t>
+  </si>
+  <si>
+    <t>new graph: with labels</t>
   </si>
 </sst>
 </file>
@@ -918,20 +913,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -947,20 +928,41 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="82">
+  <dxfs count="106">
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -987,6 +989,652 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFEB9C"/>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
       <border>
@@ -1066,411 +1714,13 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
+        <patternFill>
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1514,57 +1764,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
       <border>
@@ -2339,6 +2538,210 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2353,7 +2756,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2395,7 +2798,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2430,7 +2833,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2645,7 +3048,7 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="5.125" customWidth="1"/>
@@ -5899,19 +6302,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.125" customWidth="1"/>
     <col min="2" max="2" width="10.875" customWidth="1"/>
-    <col min="3" max="3" width="21.875" customWidth="1"/>
-    <col min="4" max="5" width="12.375" customWidth="1"/>
-    <col min="6" max="6" width="8.875" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="3" max="4" width="21.875" customWidth="1"/>
+    <col min="5" max="7" width="12.375" customWidth="1"/>
     <col min="8" max="8" width="8.875" customWidth="1"/>
     <col min="9" max="10" width="12.375" customWidth="1"/>
     <col min="11" max="11" width="36.25" customWidth="1"/>
@@ -5921,28 +6322,28 @@
     <col min="15" max="26" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="17" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -5961,10 +6362,10 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+    <row r="2" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
@@ -6227,7 +6628,7 @@
       <c r="C7" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="13">
         <v>1489</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -6461,11 +6862,9 @@
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="N11" s="16" t="s">
         <v>219</v>
       </c>
+      <c r="N11" s="16"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
@@ -6669,7 +7068,7 @@
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5" t="s">
-        <v>43</v>
+        <v>219</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -7781,7 +8180,7 @@
       <c r="C37" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="12">
         <v>1529</v>
       </c>
       <c r="E37" s="5" t="s">
@@ -8201,7 +8600,7 @@
         <v>1614</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>153</v>
+        <v>35</v>
       </c>
       <c r="F45" s="5">
         <v>509</v>
@@ -9105,7 +9504,7 @@
       </c>
       <c r="L62" s="5"/>
       <c r="M62" s="5" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
@@ -9851,7 +10250,7 @@
         <v>38</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>153</v>
+        <v>35</v>
       </c>
       <c r="J77" s="14">
         <v>42675</v>
@@ -35882,214 +36281,214 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E14:J14 D15:J31 I44:I45 I71 D46:F71 H72:I72 D73 E72:E73 D79:F80 D85:J1000 D82:E84 G84 D78:G78 F73 I73:I77 D74:F77 H46:I70 H44 D32:F44 H32:I43 D1:J13 J78:J84 J13:J28">
-    <cfRule type="containsText" dxfId="81" priority="1" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH(("Ready"),(E14))))</formula>
+  <conditionalFormatting sqref="F89:J1000 H1:J2 J3:J31 F85:H88 J78:J88">
+    <cfRule type="containsText" dxfId="93" priority="28" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(G14))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:J14 D15:J31 I44:I45 I71 D46:F71 H72:I72 D73 E72:E73 D79:F80 D85:J1000 D82:E84 G84 D78:G78 F73 I73:I77 D74:F77 H46:I70 H44 D32:F44 H32:I43 D1:J13 J78:J84 J13:J28">
-    <cfRule type="containsText" dxfId="80" priority="2" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH(("ToDo"),(E14))))</formula>
+  <conditionalFormatting sqref="F89:J1000 H1:J2 J3:J31 F85:H88 J78:J88">
+    <cfRule type="containsText" dxfId="92" priority="29" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(G14))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:J14 D15:J31 I44:I45 I71 D46:F71 H72:I72 D73 E72:E73 D79:F80 D85:J1000 D82:E84 G84 D78:G78 F73 I73:I77 D74:F77 H46:I70 H44 D32:F44 H32:I43 D1:J13 J78:J84 J13:J28">
-    <cfRule type="containsText" dxfId="79" priority="3" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH(("X"),(E14))))</formula>
+  <conditionalFormatting sqref="F89:J1000 H1:J2 J3:J31 F85:H88 J78:J88">
+    <cfRule type="containsText" dxfId="91" priority="30" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(G14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="78" priority="4" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="90" priority="31" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(K6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="89" priority="32" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(K6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="76" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="88" priority="33" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(K6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K14 K16:K1000">
-    <cfRule type="containsText" dxfId="75" priority="7" operator="containsText" text="t">
+    <cfRule type="containsText" dxfId="87" priority="34" operator="containsText" text="t">
       <formula>NOT(ISERROR(SEARCH(("t"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K14 K16:K1000">
-    <cfRule type="containsText" dxfId="74" priority="8" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="86" priority="35" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH(("esthetic differences"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K14 K16:K1000">
-    <cfRule type="cellIs" dxfId="73" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="36" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="72" priority="10" operator="containsText" text="t">
+    <cfRule type="containsText" dxfId="84" priority="37" operator="containsText" text="t">
       <formula>NOT(ISERROR(SEARCH(("t"),(K15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="71" priority="11" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="83" priority="38" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH(("esthetic differences"),(K15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="70" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="39" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="69" priority="13" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH(("Ready"),(E45))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="68" priority="14" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH(("ToDo"),(E45))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="67" priority="15" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH(("X"),(E45))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D71:F71 H71">
-    <cfRule type="containsText" dxfId="66" priority="16" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH(("Ready"),(D71))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D71:F71 H71">
-    <cfRule type="containsText" dxfId="65" priority="17" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH(("ToDo"),(D71))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D71:F71 H71">
-    <cfRule type="containsText" dxfId="64" priority="18" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH(("X"),(D71))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D73 F73">
-    <cfRule type="containsText" dxfId="63" priority="19" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH(("Ready"),(D73))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D73 F73">
-    <cfRule type="containsText" dxfId="62" priority="20" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH(("ToDo"),(D73))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D73 F73">
-    <cfRule type="containsText" dxfId="61" priority="21" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH(("X"),(D73))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E81">
-    <cfRule type="containsText" dxfId="60" priority="22" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH(("Ready"),(E81))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E81">
-    <cfRule type="containsText" dxfId="59" priority="23" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH(("ToDo"),(E81))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E81">
-    <cfRule type="containsText" dxfId="58" priority="24" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH(("X"),(E81))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G79:G83">
-    <cfRule type="containsText" dxfId="57" priority="25" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH(("Ready"),(G79))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G79:G83">
-    <cfRule type="containsText" dxfId="56" priority="26" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH(("ToDo"),(G79))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G79:G83">
-    <cfRule type="containsText" dxfId="55" priority="27" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH(("X"),(G79))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F81:F84">
-    <cfRule type="containsText" dxfId="54" priority="28" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH(("Ready"),(F81))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F81:F84">
-    <cfRule type="containsText" dxfId="53" priority="29" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH(("ToDo"),(F81))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F81:F84">
-    <cfRule type="containsText" dxfId="52" priority="30" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH(("X"),(F81))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H78:I84">
-    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH(("Ready"),(H78))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H78:I84">
-    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH(("ToDo"),(H78))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H78:I84">
-    <cfRule type="containsText" dxfId="49" priority="33" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH(("X"),(H78))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="48" priority="34" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH(("Ready"),(H73))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="47" priority="35" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH(("ToDo"),(H73))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="46" priority="36" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH(("X"),(H73))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32:G77">
-    <cfRule type="containsText" dxfId="45" priority="37" operator="containsText" text="Ready">
-      <formula>NOT(ISERROR(SEARCH(("Ready"),(G32))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32:G77">
-    <cfRule type="containsText" dxfId="44" priority="38" operator="containsText" text="ToDo">
-      <formula>NOT(ISERROR(SEARCH(("ToDo"),(G32))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32:G77">
-    <cfRule type="containsText" dxfId="43" priority="39" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH(("X"),(G32))))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J32:J77">
-    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(J32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32:J77">
-    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="65" priority="68" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(J32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32:J77">
-    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="64" priority="69" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(J32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:E1">
+    <cfRule type="containsText" dxfId="63" priority="22" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(D1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:E1">
+    <cfRule type="containsText" dxfId="62" priority="23" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(D1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:E1">
+    <cfRule type="containsText" dxfId="61" priority="24" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(D1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:E2">
+    <cfRule type="containsText" dxfId="60" priority="19" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(D2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:E2">
+    <cfRule type="containsText" dxfId="59" priority="20" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(D2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:E2">
+    <cfRule type="containsText" dxfId="58" priority="21" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(D2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F84">
+    <cfRule type="containsText" dxfId="57" priority="16" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(E3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F84">
+    <cfRule type="containsText" dxfId="56" priority="17" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(E3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F84">
+    <cfRule type="containsText" dxfId="55" priority="18" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(E3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E85:E1000">
+    <cfRule type="containsText" dxfId="44" priority="84" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(#REF!))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E85:E1000">
+    <cfRule type="containsText" dxfId="43" priority="86" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(#REF!))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E85:E1000">
+    <cfRule type="containsText" dxfId="42" priority="88" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(#REF!))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="containsText" dxfId="41" priority="13" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(F1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="containsText" dxfId="39" priority="14" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(F1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1">
+    <cfRule type="containsText" dxfId="37" priority="15" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(F1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G2">
+    <cfRule type="containsText" dxfId="35" priority="10" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(F2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G2">
+    <cfRule type="containsText" dxfId="33" priority="11" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(F2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G2">
+    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(F2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G84">
+    <cfRule type="containsText" dxfId="29" priority="7" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(G3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G84">
+    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(G3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G84">
+    <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(G3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H84">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(H3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H84">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(H3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H84">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(H3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I88">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(I3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I88">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(I3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I88">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(I3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36103,10 +36502,10 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.125" customWidth="1"/>
     <col min="2" max="2" width="10.875" customWidth="1"/>
@@ -36132,18 +36531,18 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="17" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -36510,7 +36909,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>11</v>
       </c>
@@ -36538,15 +36937,15 @@
       <c r="I9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="23" t="s">
-        <v>222</v>
+      <c r="J9" s="17" t="s">
+        <v>221</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
@@ -65439,48 +65838,63 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:J1000">
-    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="54" priority="7" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:J1000">
-    <cfRule type="containsText" dxfId="38" priority="2" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="53" priority="8" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:J1000">
-    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="52" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64:K1000">
-    <cfRule type="containsText" dxfId="36" priority="4" operator="containsText" text="Ready">
+    <cfRule type="containsText" dxfId="51" priority="10" operator="containsText" text="Ready">
       <formula>NOT(ISERROR(SEARCH(("Ready"),(K64))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64:K1000">
-    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="50" priority="11" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH(("ToDo"),(K64))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64:K1000">
-    <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="49" priority="12" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(K64))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="containsText" dxfId="33" priority="7" operator="containsText" text="t">
+    <cfRule type="containsText" dxfId="48" priority="13" operator="containsText" text="t">
       <formula>NOT(ISERROR(SEARCH(("t"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="containsText" dxfId="32" priority="8" operator="containsText" text="esthetic differences">
+    <cfRule type="containsText" dxfId="47" priority="14" operator="containsText" text="esthetic differences">
       <formula>NOT(ISERROR(SEARCH(("esthetic differences"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="15" operator="equal">
       <formula>"ok"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Ready">
+      <formula>NOT(ISERROR(SEARCH(("Ready"),(C15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="ToDo">
+      <formula>NOT(ISERROR(SEARCH(("ToDo"),(C15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH(("X"),(C15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -65492,50 +65906,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="B2" s="24" t="s">
+      <c r="A2" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="25"/>
+      <c r="E2" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="45" priority="1" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
status of matlab Codes for the first part checked!
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="227">
   <si>
     <t>Chapter</t>
   </si>
@@ -939,6 +939,9 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -952,9 +955,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5450,8 +5450,8 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5470,27 +5470,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="26" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="21" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="22"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -5510,9 +5510,9 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
@@ -9428,7 +9428,9 @@
         <v>210</v>
       </c>
       <c r="L77" s="5"/>
-      <c r="M77" s="5"/>
+      <c r="M77" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="N77" s="5"/>
       <c r="O77" s="5"/>
       <c r="P77" s="5"/>
@@ -9528,7 +9530,9 @@
         <v>43</v>
       </c>
       <c r="L79" s="5"/>
-      <c r="M79" s="5"/>
+      <c r="M79" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="N79" s="5"/>
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
@@ -9578,7 +9582,9 @@
         <v>43</v>
       </c>
       <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
+      <c r="M80" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="N80" s="5"/>
       <c r="O80" s="5"/>
       <c r="P80" s="5"/>
@@ -35700,18 +35706,18 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="26" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="21" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="22"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -65115,7 +65121,7 @@
       <c r="D2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="21">
         <v>42711</v>
       </c>
     </row>

</xml_diff>

<commit_message>
checked matlab codes of chapter 11
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="229">
   <si>
     <t>Chapter</t>
   </si>
@@ -706,7 +706,13 @@
 A Common Principal Components Approach"</t>
   </si>
   <si>
-    <t>ok, changed R Code. The fourth plot is the same as the first! Check this!</t>
+    <t>R code has a problem in the line 29, the mean value there makes no sense. Correct this when doing matlab code!</t>
+  </si>
+  <si>
+    <t>ok, changed R Code. The fourth plot is the same as the first! Ask Petra about it.</t>
+  </si>
+  <si>
+    <t>Error in Matlab Code when calculating eigenvalues and vectors</t>
   </si>
 </sst>
 </file>
@@ -760,17 +766,17 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -818,13 +824,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -906,9 +912,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -967,6 +973,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -981,15 +990,18 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="55">
@@ -5481,9 +5493,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M62" sqref="M62"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M66" sqref="M66:M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5502,27 +5514,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="27" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="22" t="s">
+      <c r="G1" s="24"/>
+      <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="23"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -5542,9 +5554,9 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
@@ -8890,7 +8902,7 @@
         <v>195</v>
       </c>
       <c r="L66" s="5"/>
-      <c r="M66" s="28" t="s">
+      <c r="M66" s="22" t="s">
         <v>223</v>
       </c>
       <c r="N66" s="5"/>
@@ -8942,7 +8954,7 @@
         <v>42</v>
       </c>
       <c r="L67" s="5"/>
-      <c r="M67" s="28" t="s">
+      <c r="M67" s="22" t="s">
         <v>224</v>
       </c>
       <c r="N67" s="5"/>
@@ -35707,9 +35719,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -35738,18 +35750,18 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="27" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="22" t="s">
+      <c r="G1" s="24"/>
+      <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="23"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -36215,7 +36227,7 @@
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="29" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -36231,7 +36243,7 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>11</v>
       </c>
@@ -36266,7 +36278,9 @@
         <v>45</v>
       </c>
       <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="M11" s="30" t="s">
+        <v>226</v>
+      </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
@@ -36316,7 +36330,9 @@
         <v>49</v>
       </c>
       <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="M12" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
@@ -36366,7 +36382,9 @@
         <v>64</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="M13" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
@@ -36416,7 +36434,9 @@
         <v>42</v>
       </c>
       <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="M14" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
@@ -36466,7 +36486,9 @@
         <v>42</v>
       </c>
       <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="M15" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
@@ -36516,7 +36538,9 @@
         <v>54</v>
       </c>
       <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="M16" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
@@ -36566,7 +36590,9 @@
         <v>74</v>
       </c>
       <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="M17" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
@@ -36616,7 +36642,9 @@
         <v>42</v>
       </c>
       <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="M18" s="31" t="s">
+        <v>228</v>
+      </c>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>

</xml_diff>

<commit_message>
comment on the last Code that was checked
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="230">
   <si>
     <t>Chapter</t>
   </si>
@@ -714,6 +714,9 @@
   <si>
     <t>R code has an error in the line 29, the mean value makes no sense. Correct this when doing matlab code! This code is imilar to the previous one.</t>
   </si>
+  <si>
+    <t>ok. I suggest to change the name of the axes.</t>
+  </si>
 </sst>
 </file>
 
@@ -988,6 +991,9 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1001,9 +1007,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5520,27 +5523,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="25" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="26"/>
+      <c r="I1" s="27"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -5560,9 +5563,9 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
@@ -35756,18 +35759,18 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="25" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="26"/>
+      <c r="I1" s="27"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -36232,7 +36235,7 @@
         <v>49</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="M10" s="31" t="s">
+      <c r="M10" s="25" t="s">
         <v>227</v>
       </c>
       <c r="N10" s="5"/>
@@ -36701,7 +36704,7 @@
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="17" t="s">
-        <v>42</v>
+        <v>229</v>
       </c>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>

</xml_diff>

<commit_message>
Matlab codes checked until chapter 16!
</commit_message>
<xml_diff>
--- a/MVA_Qlets_status.xlsx
+++ b/MVA_Qlets_status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="915" windowWidth="17655" windowHeight="5040" activeTab="2"/>
+    <workbookView xWindow="630" yWindow="915" windowWidth="13740" windowHeight="5040" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Steps" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="235">
   <si>
     <t>Chapter</t>
   </si>
@@ -717,12 +717,27 @@
   <si>
     <t>ok. I suggest to change the name of the axes.</t>
   </si>
+  <si>
+    <t>Matlab code doesn't produce the plot with the groups.</t>
+  </si>
+  <si>
+    <t>Matlab code only produces the plot of the dendogram and omit the other two.</t>
+  </si>
+  <si>
+    <t>ok, modified R code</t>
+  </si>
+  <si>
+    <t>Matlab Code doesn't work</t>
+  </si>
+  <si>
+    <t>ok, I changed the tittle of the plots from R and Matlab but not of the one from SAS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -786,6 +801,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -923,7 +949,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -994,6 +1020,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,6 +1039,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5523,27 +5558,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="31" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="26" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="27"/>
+      <c r="I1" s="29"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -5563,9 +5598,9 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
@@ -35728,9 +35763,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -35759,18 +35794,18 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="31" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="26" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="27"/>
+      <c r="I1" s="29"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -36755,7 +36790,9 @@
         <v>54</v>
       </c>
       <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="M20" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
@@ -36805,7 +36842,9 @@
         <v>84</v>
       </c>
       <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="M21" s="26" t="s">
+        <v>230</v>
+      </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
@@ -36820,7 +36859,7 @@
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>13</v>
       </c>
@@ -36855,7 +36894,9 @@
         <v>42</v>
       </c>
       <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="M22" s="27" t="s">
+        <v>231</v>
+      </c>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -36905,7 +36946,9 @@
         <v>42</v>
       </c>
       <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="M23" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
@@ -36955,7 +36998,9 @@
         <v>49</v>
       </c>
       <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
+      <c r="M24" s="5" t="s">
+        <v>232</v>
+      </c>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
@@ -37005,7 +37050,9 @@
         <v>92</v>
       </c>
       <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
+      <c r="M25" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
@@ -37055,7 +37102,9 @@
         <v>42</v>
       </c>
       <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
+      <c r="M26" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
@@ -37105,7 +37154,9 @@
         <v>99</v>
       </c>
       <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
+      <c r="M27" s="26" t="s">
+        <v>233</v>
+      </c>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
@@ -37155,7 +37206,9 @@
         <v>102</v>
       </c>
       <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
+      <c r="M28" s="26" t="s">
+        <v>233</v>
+      </c>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
@@ -37205,7 +37258,9 @@
         <v>45</v>
       </c>
       <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
+      <c r="M29" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
@@ -37255,7 +37310,9 @@
         <v>109</v>
       </c>
       <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
+      <c r="M30" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
@@ -37270,7 +37327,7 @@
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>15</v>
       </c>
@@ -37305,7 +37362,9 @@
         <v>45</v>
       </c>
       <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
+      <c r="M31" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
@@ -37320,7 +37379,7 @@
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>16</v>
       </c>
@@ -37355,7 +37414,9 @@
         <v>81</v>
       </c>
       <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
+      <c r="M32" s="34" t="s">
+        <v>234</v>
+      </c>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>

</xml_diff>